<commit_message>
modified:   cadastro_turmas.xlsx 	modified:   main.py 	modified:   mofome.kv
</commit_message>
<xml_diff>
--- a/cadastro_turmas.xlsx
+++ b/cadastro_turmas.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -492,6 +492,16 @@
         <v>1203945</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2AADM</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1093985</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>